<commit_message>
add func laporan lipa 7b
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_7a.xlsx
+++ b/hasil/2023_01_lipa_7a.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>LAPORAN KEUANGAN PERKARA</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Saldo Awal</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Penerimaan Bulan ini</t>
   </si>
   <si>
@@ -119,7 +116,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 11 Agustus 2023</t>
+    <t>Ternate , 15 Agustus 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -148,7 +145,7 @@
     <numFmt numFmtId="164" formatCode="_([$Rp-421]* #,##0_);_([$Rp-421]* \(#,##0\);_([$Rp-421]* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-[$Rp-421]* #,##0.00_-;\-[$Rp-421]* #,##0.00_-;_-[$Rp-421]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -203,6 +200,24 @@
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -364,6 +379,34 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="5" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
@@ -372,103 +415,75 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="5" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="164" fillId="2" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="7" numFmtId="164" fillId="2" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="164" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="7" numFmtId="164" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="164" fillId="2" borderId="4" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="165" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="164" fillId="2" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="165" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="7" numFmtId="164" fillId="2" borderId="4" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="165" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="164" fillId="2" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="165" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="165" fillId="2" borderId="6" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="7" numFmtId="165" fillId="2" borderId="6" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="164" fillId="2" borderId="7" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="6" numFmtId="164" fillId="2" borderId="7" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="165" fillId="2" borderId="6" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="7" numFmtId="165" fillId="2" borderId="6" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
@@ -799,28 +814,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" customHeight="1" ht="15.6">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:8" customHeight="1" ht="15.6">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:8" customHeight="1" ht="15.6">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:8" customHeight="1" ht="14.4">
       <c r="B4" s="1"/>
@@ -831,48 +846,48 @@
       </c>
     </row>
     <row r="5" spans="1:8" customHeight="1" ht="15">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:8" customHeight="1" ht="15">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" customHeight="1" ht="15">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="10" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" customHeight="1" ht="15">
-      <c r="B8" s="11">
+      <c r="B8" s="9">
         <v>1</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>2</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>3</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="9">
         <v>4</v>
       </c>
     </row>
@@ -886,34 +901,28 @@
       <c r="D9" s="21">
         <v>219276300</v>
       </c>
-      <c r="E9" s="23" t="s">
-        <v>11</v>
-      </c>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:8" customHeight="1" ht="18">
       <c r="B10" s="27">
         <v>2</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="21">
         <v>90120000</v>
       </c>
-      <c r="E10" s="23" t="s">
-        <v>11</v>
-      </c>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:8" customHeight="1" ht="18">
       <c r="B11" s="27">
         <v>3</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D11" s="21"/>
       <c r="E11" s="23">
         <v>9800000</v>
       </c>
@@ -923,11 +932,9 @@
         <v>4</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D12" s="21"/>
       <c r="E12" s="23">
         <v>31420000</v>
       </c>
@@ -937,11 +944,9 @@
         <v>5</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D13" s="21"/>
       <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:8" customHeight="1" ht="18">
@@ -949,11 +954,9 @@
         <v>6</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D14" s="21"/>
       <c r="E14" s="23">
         <v>6910000</v>
       </c>
@@ -963,11 +966,9 @@
         <v>7</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D15" s="21"/>
       <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:8" customHeight="1" ht="18">
@@ -975,11 +976,9 @@
         <v>8</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D16" s="21"/>
       <c r="E16" s="23"/>
       <c r="H16" s="2"/>
     </row>
@@ -988,11 +987,9 @@
         <v>9</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D17" s="21"/>
       <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:8" customHeight="1" ht="18">
@@ -1000,11 +997,9 @@
         <v>10</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D18" s="21"/>
       <c r="E18" s="23">
         <v>960600</v>
       </c>
@@ -1014,11 +1009,9 @@
         <v>11</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D19" s="21"/>
       <c r="E19" s="23">
         <v>590000</v>
       </c>
@@ -1028,7 +1021,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="23"/>
@@ -1036,11 +1029,9 @@
     <row r="21" spans="1:8" customHeight="1" ht="18">
       <c r="B21" s="27"/>
       <c r="C21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D21" s="21"/>
       <c r="E21" s="23">
         <v>2340000</v>
       </c>
@@ -1048,25 +1039,21 @@
     <row r="22" spans="1:8" customHeight="1" ht="18">
       <c r="B22" s="27"/>
       <c r="C22" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>11</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D22" s="21"/>
       <c r="E22" s="23">
         <v>2990000</v>
       </c>
     </row>
     <row r="23" spans="1:8" customHeight="1" ht="18">
       <c r="B23" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>11</v>
-      </c>
+      <c r="D23" s="21"/>
       <c r="E23" s="23">
         <v>590000</v>
       </c>
@@ -1076,21 +1063,19 @@
         <v>13</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>11</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D24" s="32"/>
       <c r="E24" s="24">
         <v>62817000</v>
       </c>
     </row>
     <row r="25" spans="1:8" customHeight="1" ht="18">
       <c r="B25" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="22">
         <v>309396300</v>
@@ -1100,28 +1085,28 @@
       </c>
     </row>
     <row r="26" spans="1:8" customHeight="1" ht="18">
-      <c r="B26" s="12"/>
-      <c r="C26" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="14" t="str">
+      <c r="B26" s="10"/>
+      <c r="C26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="16" t="str">
         <f>D25-E25</f>
         <v>0</v>
       </c>
-      <c r="E26" s="14"/>
+      <c r="E26" s="16"/>
     </row>
     <row r="27" spans="1:8" customHeight="1" ht="18">
-      <c r="B27" s="15"/>
-      <c r="C27" s="16" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+    </row>
+    <row r="28" spans="1:8" customHeight="1" ht="18">
+      <c r="B28" s="12"/>
+      <c r="C28" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-    </row>
-    <row r="28" spans="1:8" customHeight="1" ht="18">
-      <c r="B28" s="18"/>
-      <c r="C28" s="19" t="s">
-        <v>31</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -1129,21 +1114,21 @@
     <row r="29" spans="1:8" customHeight="1" ht="20">
       <c r="B29" s="4"/>
       <c r="C29" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="33"/>
       <c r="E29" s="33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:8" customHeight="1" ht="20">
       <c r="B30" s="4"/>
       <c r="C30" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="34"/>
       <c r="E30" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:8" customHeight="1" ht="15">
@@ -1173,21 +1158,21 @@
     <row r="35" spans="1:8" customHeight="1" ht="20">
       <c r="B35" s="4"/>
       <c r="C35" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:8" customHeight="1" ht="20">
       <c r="B36" s="4"/>
       <c r="C36" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" s="33"/>
       <c r="E36" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:8" customHeight="1" ht="14.4">

</xml_diff>

<commit_message>
add env to the project
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_7a.xlsx
+++ b/hasil/2023_01_lipa_7a.xlsx
@@ -116,7 +116,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 15 Agustus 2023</t>
+    <t>Ternate , 29 Agustus 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -947,7 +947,9 @@
         <v>14</v>
       </c>
       <c r="D13" s="21"/>
-      <c r="E13" s="23"/>
+      <c r="E13" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" customHeight="1" ht="18">
       <c r="B14" s="27">
@@ -969,7 +971,9 @@
         <v>16</v>
       </c>
       <c r="D15" s="21"/>
-      <c r="E15" s="23"/>
+      <c r="E15" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8" customHeight="1" ht="18">
       <c r="B16" s="27">
@@ -979,7 +983,9 @@
         <v>17</v>
       </c>
       <c r="D16" s="21"/>
-      <c r="E16" s="23"/>
+      <c r="E16" s="23">
+        <v>0</v>
+      </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" customHeight="1" ht="18">
@@ -990,7 +996,9 @@
         <v>18</v>
       </c>
       <c r="D17" s="21"/>
-      <c r="E17" s="23"/>
+      <c r="E17" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:8" customHeight="1" ht="18">
       <c r="B18" s="27">

</xml_diff>